<commit_message>
plots done? and got some real results
</commit_message>
<xml_diff>
--- a/results/FP sqrt_sum Mar_23_11.18.29/results1.xlsx
+++ b/results/FP sqrt_sum Mar_23_11.18.29/results1.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felipenoris/tmp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonathan\git\python\results\FP sqrt_sum Mar_23_11.18.29\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C353BCB8-5EC8-0143-BDD3-A1B661DAACD7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324AF816-DF4B-47C4-B80A-5A002DC049E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
+    <workbookView xWindow="10290" yWindow="0" windowWidth="9825" windowHeight="21000" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
   </bookViews>
   <sheets>
     <sheet name="Results 180 s" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Results 180 s'!$A$1:$D$43</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="91">
   <si>
     <t>Combination</t>
   </si>
@@ -651,11 +654,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="B1:D43"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.25" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -669,21 +677,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="B2">
-        <v>106774.19069631507</v>
+        <v>112238.01554931488</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -697,539 +705,539 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4">
+        <v>112502.81654952877</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5">
+        <v>110955.29324186414</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6">
+        <v>111268.87634359101</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7">
+        <v>112722.19363347157</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>106774.19069631507</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9">
+        <v>113564.17741592694</v>
+      </c>
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10">
+        <v>119993.46384723061</v>
+      </c>
+      <c r="C10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11">
+        <v>116991.66346861421</v>
+      </c>
+      <c r="C11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12">
+        <v>118509.00625238546</v>
+      </c>
+      <c r="C12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>109139.05139879946</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14">
+        <v>109488.24954415119</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>10</v>
       </c>
-      <c r="B4">
+      <c r="B15">
         <v>108393.00941120317</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C15" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5">
-        <v>108558.37263280839</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6">
-        <v>108672.37850652286</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7">
-        <v>108772.11186658806</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>108823.66614899007</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17">
+        <v>114519.71506016477</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18">
+        <v>117258.61372917719</v>
+      </c>
+      <c r="C18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19">
+        <v>115234.62735530884</v>
+      </c>
+      <c r="C19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20">
+        <v>119349.39301943393</v>
+      </c>
+      <c r="C20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8">
-        <v>108823.66614899007</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9">
-        <v>109139.05139879946</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10">
-        <v>109488.24954415119</v>
-      </c>
-      <c r="C10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21">
+        <v>125210.65455372073</v>
+      </c>
+      <c r="C21" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22">
+        <v>120326.33546438489</v>
+      </c>
+      <c r="C22" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23">
+        <v>112820.35065150396</v>
+      </c>
+      <c r="C23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>25</v>
       </c>
-      <c r="B11">
+      <c r="B24">
         <v>110478.28709560526</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C24" t="s">
         <v>26</v>
-      </c>
-      <c r="D11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12">
-        <v>110955.29324186414</v>
-      </c>
-      <c r="C12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13">
-        <v>111268.87634359101</v>
-      </c>
-      <c r="C13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14">
-        <v>111536.17422323994</v>
-      </c>
-      <c r="C14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15">
-        <v>111892.13937837652</v>
-      </c>
-      <c r="C15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16">
-        <v>112238.01554931488</v>
-      </c>
-      <c r="C16" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17">
-        <v>112502.81654952877</v>
-      </c>
-      <c r="C17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18">
-        <v>112722.19363347157</v>
-      </c>
-      <c r="C18" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19">
-        <v>112820.35065150396</v>
-      </c>
-      <c r="C19" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20">
-        <v>112830.15965083461</v>
-      </c>
-      <c r="C20" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
-        <v>45</v>
-      </c>
-      <c r="B21">
-        <v>113136.96556303307</v>
-      </c>
-      <c r="C21" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" t="s">
-        <v>47</v>
-      </c>
-      <c r="B22">
-        <v>113193.66944412493</v>
-      </c>
-      <c r="C22" t="s">
-        <v>48</v>
-      </c>
-      <c r="D22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23">
-        <v>113564.17741592694</v>
-      </c>
-      <c r="C23" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24">
-        <v>114288.91851134085</v>
-      </c>
-      <c r="C24" t="s">
-        <v>52</v>
       </c>
       <c r="D24" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B25">
-        <v>114519.71506016477</v>
+        <v>114764.47368588163</v>
       </c>
       <c r="C25" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B26">
-        <v>114764.47368588163</v>
+        <v>113193.66944412493</v>
       </c>
       <c r="C26" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D26" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B27">
-        <v>115234.62735530884</v>
+        <v>113136.96556303307</v>
       </c>
       <c r="C27" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="D27" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28">
+        <v>112830.15965083461</v>
+      </c>
+      <c r="C28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29">
+        <v>108672.37850652286</v>
+      </c>
+      <c r="C29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30">
+        <v>114288.91851134085</v>
+      </c>
+      <c r="C30" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31">
+        <v>121538.03628091504</v>
+      </c>
+      <c r="C31" t="s">
+        <v>86</v>
+      </c>
+      <c r="D31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32">
+        <v>118632.24918160478</v>
+      </c>
+      <c r="C32" t="s">
+        <v>72</v>
+      </c>
+      <c r="D32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33">
+        <v>117775.7374161757</v>
+      </c>
+      <c r="C33" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34">
+        <v>111536.17422323994</v>
+      </c>
+      <c r="C34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35">
+        <v>108772.11186658806</v>
+      </c>
+      <c r="C35" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36">
+        <v>111892.13937837652</v>
+      </c>
+      <c r="C36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37">
+        <v>108558.37263280839</v>
+      </c>
+      <c r="C37" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>59</v>
       </c>
-      <c r="B28">
+      <c r="B38">
         <v>116496.24829179514</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C38" t="s">
         <v>60</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D38" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
-      <c r="A29" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39">
+        <v>118740.76069277126</v>
+      </c>
+      <c r="C39" t="s">
+        <v>74</v>
+      </c>
+      <c r="D39" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>61</v>
       </c>
-      <c r="B29">
+      <c r="B40">
         <v>116750.58321966483</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C40" t="s">
         <v>62</v>
       </c>
-      <c r="D29" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" t="s">
-        <v>63</v>
-      </c>
-      <c r="B30">
-        <v>116991.6634686142</v>
-      </c>
-      <c r="C30" t="s">
-        <v>64</v>
-      </c>
-      <c r="D30" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" t="s">
-        <v>65</v>
-      </c>
-      <c r="B31">
-        <v>117258.61372917719</v>
-      </c>
-      <c r="C31" t="s">
-        <v>66</v>
-      </c>
-      <c r="D31" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" t="s">
-        <v>67</v>
-      </c>
-      <c r="B32">
-        <v>117775.7374161757</v>
-      </c>
-      <c r="C32" t="s">
-        <v>68</v>
-      </c>
-      <c r="D32" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" t="s">
-        <v>69</v>
-      </c>
-      <c r="B33">
-        <v>118509.00625238546</v>
-      </c>
-      <c r="C33" t="s">
-        <v>70</v>
-      </c>
-      <c r="D33" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" t="s">
-        <v>71</v>
-      </c>
-      <c r="B34">
-        <v>118632.24918160478</v>
-      </c>
-      <c r="C34" t="s">
-        <v>72</v>
-      </c>
-      <c r="D34" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" t="s">
-        <v>73</v>
-      </c>
-      <c r="B35">
-        <v>118740.76069277126</v>
-      </c>
-      <c r="C35" t="s">
-        <v>74</v>
-      </c>
-      <c r="D35" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" t="s">
-        <v>75</v>
-      </c>
-      <c r="B36">
-        <v>119349.39301943393</v>
-      </c>
-      <c r="C36" t="s">
-        <v>76</v>
-      </c>
-      <c r="D36" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" t="s">
-        <v>77</v>
-      </c>
-      <c r="B37">
-        <v>119993.46384723061</v>
-      </c>
-      <c r="C37" t="s">
-        <v>78</v>
-      </c>
-      <c r="D37" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" t="s">
+      <c r="D40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>79</v>
       </c>
-      <c r="B38">
+      <c r="B41">
         <v>120238.87556768175</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C41" t="s">
         <v>80</v>
       </c>
-      <c r="D38" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" t="s">
-        <v>81</v>
-      </c>
-      <c r="B39">
-        <v>120299.57166900966</v>
-      </c>
-      <c r="C39" t="s">
-        <v>82</v>
-      </c>
-      <c r="D39" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" t="s">
-        <v>83</v>
-      </c>
-      <c r="B40">
-        <v>120326.33546438489</v>
-      </c>
-      <c r="C40" t="s">
-        <v>84</v>
-      </c>
-      <c r="D40" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" t="s">
-        <v>85</v>
-      </c>
-      <c r="B41">
-        <v>121538.03628091504</v>
-      </c>
-      <c r="C41" t="s">
-        <v>86</v>
-      </c>
       <c r="D41" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>87</v>
       </c>
@@ -1243,21 +1251,38 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B43">
-        <v>125210.65455372073</v>
+        <v>120299.57166900966</v>
       </c>
       <c r="C43" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D43" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D43" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D43">
+      <sortCondition ref="A1:A43"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>